<commit_message>
whoops forgot to save one of the excel files
</commit_message>
<xml_diff>
--- a/tim/part1/violations_grouped_by_category.xlsx
+++ b/tim/part1/violations_grouped_by_category.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="16400" tabRatio="500"/>
+    <workbookView xWindow="6640" yWindow="1320" windowWidth="25120" windowHeight="16400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="top_violations_grouped_by_categ" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,22 +19,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>violation_category</t>
   </si>
   <si>
     <t>count</t>
   </si>
+  <si>
+    <t>All issuers</t>
+  </si>
+  <si>
+    <t>Top performers only</t>
+  </si>
+  <si>
+    <t>rel %</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -57,13 +82,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -393,70 +427,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>83477</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
+      <c r="C3" s="1">
+        <f>B3/SUM($B$3:$B$8)</f>
+        <v>0.10321960797891019</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>166861</v>
+      </c>
+      <c r="G3" s="1">
+        <f>F3/SUM($F$3:$F$9)</f>
+        <v>8.0998951961589072E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>395737</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:C8" si="0">B4/SUM($B$3:$B$8)</f>
+        <v>0.48933021074966737</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>896413</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" ref="G4:G9" si="1">F4/SUM($F$3:$F$9)</f>
+        <v>0.43514370359007765</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>85510</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10573341972371564</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>229500</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.11140565785405034</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>64309</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>7.9518307671762711E-2</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>221699</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.10761883634241876</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>176954</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.21880425159385308</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>535962</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.26017080259160141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>2745</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3942022820909771E-3</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>9273</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>4.501371090547315E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="F9">
+        <v>331</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6067656971542772E-4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>